<commit_message>
feat(page_rp): add sim for opt in random seqnence
add sim for opt algorithm in random seqnence
add a paper (unread)
todo : analyze expect miss ratio for random sequence
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljt12138\Desktop\oslab\sim_ran\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljt12138\Desktop\oslab\sim_ran\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A74A8-970A-4E02-912E-E2024C29455B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1728F447-45D0-46F6-90FF-CE6089398F10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{5F17E777-6804-43E9-9C86-08DF6650385B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{5F17E777-6804-43E9-9C86-08DF6650385B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Push</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +54,14 @@
   </si>
   <si>
     <t>Rat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>miss ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frame</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7681,6 +7690,1022 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$B$1:$DX$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="127"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>364</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>508</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$DX$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="127"/>
+                <c:pt idx="0">
+                  <c:v>0.86499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.63900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.57799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.56399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.55100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.53900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.51600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.49399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.45200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.443</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.433</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.42399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.40699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.39900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.38300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.376</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.36899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.35199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.34399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.33600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.33300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.32500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.318</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.29599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.29199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.28499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.27900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.27200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.26700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.26300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.251</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.247</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.23400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.219</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.215</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.20899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.19800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.186</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.182</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.17100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.16700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.16300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.151</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.14399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.13300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.113</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.107</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.104</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9.0999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8.5000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>8.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7.2999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>7.0999999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5.7000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7F4D-44BD-822F-6E40BDBC3A04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="575153208"/>
+        <c:axId val="575156408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="575153208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="575156408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="575156408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="575153208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7802,6 +8827,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9905,6 +10970,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10055,6 +11636,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5CE5847-1509-4C50-A563-2180A81A0441}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10362,8 +11984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB92DB3-3B0C-4093-9EA3-9D941B05C09F}">
   <dimension ref="A1:DX6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="X55" sqref="X55"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -14515,4 +16137,794 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD326260-283E-4D7E-BA0A-A1AA4C1E2C9B}">
+  <dimension ref="A1:DX2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:128" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <v>16</v>
+      </c>
+      <c r="F1">
+        <v>20</v>
+      </c>
+      <c r="G1">
+        <v>24</v>
+      </c>
+      <c r="H1">
+        <v>28</v>
+      </c>
+      <c r="I1">
+        <v>32</v>
+      </c>
+      <c r="J1">
+        <v>36</v>
+      </c>
+      <c r="K1">
+        <v>40</v>
+      </c>
+      <c r="L1">
+        <v>44</v>
+      </c>
+      <c r="M1">
+        <v>48</v>
+      </c>
+      <c r="N1">
+        <v>52</v>
+      </c>
+      <c r="O1">
+        <v>56</v>
+      </c>
+      <c r="P1">
+        <v>60</v>
+      </c>
+      <c r="Q1">
+        <v>64</v>
+      </c>
+      <c r="R1">
+        <v>68</v>
+      </c>
+      <c r="S1">
+        <v>72</v>
+      </c>
+      <c r="T1">
+        <v>76</v>
+      </c>
+      <c r="U1">
+        <v>80</v>
+      </c>
+      <c r="V1">
+        <v>84</v>
+      </c>
+      <c r="W1">
+        <v>88</v>
+      </c>
+      <c r="X1">
+        <v>92</v>
+      </c>
+      <c r="Y1">
+        <v>96</v>
+      </c>
+      <c r="Z1">
+        <v>100</v>
+      </c>
+      <c r="AA1">
+        <v>104</v>
+      </c>
+      <c r="AB1">
+        <v>108</v>
+      </c>
+      <c r="AC1">
+        <v>112</v>
+      </c>
+      <c r="AD1">
+        <v>116</v>
+      </c>
+      <c r="AE1">
+        <v>120</v>
+      </c>
+      <c r="AF1">
+        <v>124</v>
+      </c>
+      <c r="AG1">
+        <v>128</v>
+      </c>
+      <c r="AH1">
+        <v>132</v>
+      </c>
+      <c r="AI1">
+        <v>136</v>
+      </c>
+      <c r="AJ1">
+        <v>140</v>
+      </c>
+      <c r="AK1">
+        <v>144</v>
+      </c>
+      <c r="AL1">
+        <v>148</v>
+      </c>
+      <c r="AM1">
+        <v>152</v>
+      </c>
+      <c r="AN1">
+        <v>156</v>
+      </c>
+      <c r="AO1">
+        <v>160</v>
+      </c>
+      <c r="AP1">
+        <v>164</v>
+      </c>
+      <c r="AQ1">
+        <v>168</v>
+      </c>
+      <c r="AR1">
+        <v>172</v>
+      </c>
+      <c r="AS1">
+        <v>176</v>
+      </c>
+      <c r="AT1">
+        <v>180</v>
+      </c>
+      <c r="AU1">
+        <v>184</v>
+      </c>
+      <c r="AV1">
+        <v>188</v>
+      </c>
+      <c r="AW1">
+        <v>192</v>
+      </c>
+      <c r="AX1">
+        <v>196</v>
+      </c>
+      <c r="AY1">
+        <v>200</v>
+      </c>
+      <c r="AZ1">
+        <v>204</v>
+      </c>
+      <c r="BA1">
+        <v>208</v>
+      </c>
+      <c r="BB1">
+        <v>212</v>
+      </c>
+      <c r="BC1">
+        <v>216</v>
+      </c>
+      <c r="BD1">
+        <v>220</v>
+      </c>
+      <c r="BE1">
+        <v>224</v>
+      </c>
+      <c r="BF1">
+        <v>228</v>
+      </c>
+      <c r="BG1">
+        <v>232</v>
+      </c>
+      <c r="BH1">
+        <v>236</v>
+      </c>
+      <c r="BI1">
+        <v>240</v>
+      </c>
+      <c r="BJ1">
+        <v>244</v>
+      </c>
+      <c r="BK1">
+        <v>248</v>
+      </c>
+      <c r="BL1">
+        <v>252</v>
+      </c>
+      <c r="BM1">
+        <v>256</v>
+      </c>
+      <c r="BN1">
+        <v>260</v>
+      </c>
+      <c r="BO1">
+        <v>264</v>
+      </c>
+      <c r="BP1">
+        <v>268</v>
+      </c>
+      <c r="BQ1">
+        <v>272</v>
+      </c>
+      <c r="BR1">
+        <v>276</v>
+      </c>
+      <c r="BS1">
+        <v>280</v>
+      </c>
+      <c r="BT1">
+        <v>284</v>
+      </c>
+      <c r="BU1">
+        <v>288</v>
+      </c>
+      <c r="BV1">
+        <v>292</v>
+      </c>
+      <c r="BW1">
+        <v>296</v>
+      </c>
+      <c r="BX1">
+        <v>300</v>
+      </c>
+      <c r="BY1">
+        <v>304</v>
+      </c>
+      <c r="BZ1">
+        <v>308</v>
+      </c>
+      <c r="CA1">
+        <v>312</v>
+      </c>
+      <c r="CB1">
+        <v>316</v>
+      </c>
+      <c r="CC1">
+        <v>320</v>
+      </c>
+      <c r="CD1">
+        <v>324</v>
+      </c>
+      <c r="CE1">
+        <v>328</v>
+      </c>
+      <c r="CF1">
+        <v>332</v>
+      </c>
+      <c r="CG1">
+        <v>336</v>
+      </c>
+      <c r="CH1">
+        <v>340</v>
+      </c>
+      <c r="CI1">
+        <v>344</v>
+      </c>
+      <c r="CJ1">
+        <v>348</v>
+      </c>
+      <c r="CK1">
+        <v>352</v>
+      </c>
+      <c r="CL1">
+        <v>356</v>
+      </c>
+      <c r="CM1">
+        <v>360</v>
+      </c>
+      <c r="CN1">
+        <v>364</v>
+      </c>
+      <c r="CO1">
+        <v>368</v>
+      </c>
+      <c r="CP1">
+        <v>372</v>
+      </c>
+      <c r="CQ1">
+        <v>376</v>
+      </c>
+      <c r="CR1">
+        <v>380</v>
+      </c>
+      <c r="CS1">
+        <v>384</v>
+      </c>
+      <c r="CT1">
+        <v>388</v>
+      </c>
+      <c r="CU1">
+        <v>392</v>
+      </c>
+      <c r="CV1">
+        <v>396</v>
+      </c>
+      <c r="CW1">
+        <v>400</v>
+      </c>
+      <c r="CX1">
+        <v>404</v>
+      </c>
+      <c r="CY1">
+        <v>408</v>
+      </c>
+      <c r="CZ1">
+        <v>412</v>
+      </c>
+      <c r="DA1">
+        <v>416</v>
+      </c>
+      <c r="DB1">
+        <v>420</v>
+      </c>
+      <c r="DC1">
+        <v>424</v>
+      </c>
+      <c r="DD1">
+        <v>428</v>
+      </c>
+      <c r="DE1">
+        <v>432</v>
+      </c>
+      <c r="DF1">
+        <v>436</v>
+      </c>
+      <c r="DG1">
+        <v>440</v>
+      </c>
+      <c r="DH1">
+        <v>444</v>
+      </c>
+      <c r="DI1">
+        <v>448</v>
+      </c>
+      <c r="DJ1">
+        <v>452</v>
+      </c>
+      <c r="DK1">
+        <v>456</v>
+      </c>
+      <c r="DL1">
+        <v>460</v>
+      </c>
+      <c r="DM1">
+        <v>464</v>
+      </c>
+      <c r="DN1">
+        <v>468</v>
+      </c>
+      <c r="DO1">
+        <v>472</v>
+      </c>
+      <c r="DP1">
+        <v>476</v>
+      </c>
+      <c r="DQ1">
+        <v>480</v>
+      </c>
+      <c r="DR1">
+        <v>484</v>
+      </c>
+      <c r="DS1">
+        <v>488</v>
+      </c>
+      <c r="DT1">
+        <v>492</v>
+      </c>
+      <c r="DU1">
+        <v>496</v>
+      </c>
+      <c r="DV1">
+        <v>500</v>
+      </c>
+      <c r="DW1">
+        <v>504</v>
+      </c>
+      <c r="DX1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:128" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D2">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="E2">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="H2">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="I2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="J2">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="K2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="L2">
+        <v>0.625</v>
+      </c>
+      <c r="M2">
+        <v>0.61</v>
+      </c>
+      <c r="N2">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="O2">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="P2">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="Q2">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="R2">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="S2">
+        <v>0.53</v>
+      </c>
+      <c r="T2">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="U2">
+        <v>0.505</v>
+      </c>
+      <c r="V2">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="W2">
+        <v>0.48</v>
+      </c>
+      <c r="X2">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="Y2">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="Z2">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="AA2">
+        <v>0.443</v>
+      </c>
+      <c r="AB2">
+        <v>0.433</v>
+      </c>
+      <c r="AC2">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="AD2">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="AE2">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="AF2">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="AG2">
+        <v>0.39</v>
+      </c>
+      <c r="AH2">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="AI2">
+        <v>0.376</v>
+      </c>
+      <c r="AJ2">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="AK2">
+        <v>0.36</v>
+      </c>
+      <c r="AL2">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="AM2">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="AN2">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="AO2">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="AP2">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="AQ2">
+        <v>0.318</v>
+      </c>
+      <c r="AR2">
+        <v>0.31</v>
+      </c>
+      <c r="AS2">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="AT2">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="AU2">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="AV2">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AW2">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="AX2">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AY2">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="AZ2">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="BA2">
+        <v>0.254</v>
+      </c>
+      <c r="BB2">
+        <v>0.251</v>
+      </c>
+      <c r="BC2">
+        <v>0.247</v>
+      </c>
+      <c r="BD2">
+        <v>0.24</v>
+      </c>
+      <c r="BE2">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="BF2">
+        <v>0.23</v>
+      </c>
+      <c r="BG2">
+        <v>0.222</v>
+      </c>
+      <c r="BH2">
+        <v>0.219</v>
+      </c>
+      <c r="BI2">
+        <v>0.215</v>
+      </c>
+      <c r="BJ2">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="BK2">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="BL2">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="BM2">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="BN2">
+        <v>0.19</v>
+      </c>
+      <c r="BO2">
+        <v>0.186</v>
+      </c>
+      <c r="BP2">
+        <v>0.182</v>
+      </c>
+      <c r="BQ2">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="BR2">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="BS2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="BT2">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="BU2">
+        <v>0.158</v>
+      </c>
+      <c r="BV2">
+        <v>0.156</v>
+      </c>
+      <c r="BW2">
+        <v>0.151</v>
+      </c>
+      <c r="BX2">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="BY2">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="BZ2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="CA2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="CB2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="CC2">
+        <v>0.128</v>
+      </c>
+      <c r="CD2">
+        <v>0.125</v>
+      </c>
+      <c r="CE2">
+        <v>0.121</v>
+      </c>
+      <c r="CF2">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="CG2">
+        <v>0.113</v>
+      </c>
+      <c r="CH2">
+        <v>0.111</v>
+      </c>
+      <c r="CI2">
+        <v>0.107</v>
+      </c>
+      <c r="CJ2">
+        <v>0.104</v>
+      </c>
+      <c r="CK2">
+        <v>0.1</v>
+      </c>
+      <c r="CL2">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="CM2">
+        <v>9.4E-2</v>
+      </c>
+      <c r="CN2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="CO2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="CP2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="CQ2">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="CR2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="CS2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="CT2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="CU2">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="CV2">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="CW2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="CX2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="CY2">
+        <v>0.06</v>
+      </c>
+      <c r="CZ2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="DA2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="DB2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="DC2">
+        <v>0.05</v>
+      </c>
+      <c r="DD2">
+        <v>4.7E-2</v>
+      </c>
+      <c r="DE2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="DF2">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="DG2">
+        <v>0.04</v>
+      </c>
+      <c r="DH2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="DI2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="DJ2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="DK2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="DL2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="DM2">
+        <v>2.7E-2</v>
+      </c>
+      <c r="DN2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="DO2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="DP2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="DQ2">
+        <v>0.02</v>
+      </c>
+      <c r="DR2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="DS2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="DT2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="DU2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="DV2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="DW2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="DX2">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs(paper): add a paper
a paper about math model for locality
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljt12138\Desktop\oslab\sim_ran\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1728F447-45D0-46F6-90FF-CE6089398F10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1324A57A-7404-4C36-8075-9F3EE34966B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{5F17E777-6804-43E9-9C86-08DF6650385B}"/>
   </bookViews>
@@ -259,8 +259,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.7736550088894301E-2"/>
-                  <c:y val="-0.10603701976327144"/>
+                  <c:x val="-6.2566596773903999E-2"/>
+                  <c:y val="-0.11251976920558909"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1123,8 +1123,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.0097441027585864E-2"/>
-                  <c:y val="9.9170234169753259E-4"/>
+                  <c:x val="-0.11444248686130441"/>
+                  <c:y val="-1.6423998604616106E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -11649,15 +11649,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11985,7 +11985,7 @@
   <dimension ref="A1:DX6"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -16141,15 +16141,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD326260-283E-4D7E-BA0A-A1AA4C1E2C9B}">
-  <dimension ref="A1:DX2"/>
+  <dimension ref="A1:DY3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:128" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:129" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -16535,7 +16535,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="2" spans="1:128" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:129" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -16919,6 +16919,392 @@
       </c>
       <c r="DX2">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:129" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="D3">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="E3">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="F3">
+        <v>0.753</v>
+      </c>
+      <c r="G3">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="H3">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="I3">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="J3">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="K3">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="L3">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N3">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="O3">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="P3">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="Q3">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="R3">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="S3">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="T3">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="U3">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="V3">
+        <v>0.499</v>
+      </c>
+      <c r="W3">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="X3">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="Y3">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="Z3">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="AA3">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="AB3">
+        <v>0.442</v>
+      </c>
+      <c r="AC3">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="AD3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="AE3">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="AF3">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="AG3">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="AH3">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="AI3">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="AJ3">
+        <v>0.374</v>
+      </c>
+      <c r="AK3">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="AL3">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="AM3">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="AN3">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="AO3">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="AP3">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="AQ3">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AR3">
+        <v>0.317</v>
+      </c>
+      <c r="AS3">
+        <v>0.312</v>
+      </c>
+      <c r="AT3">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="AU3">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="AV3">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AW3">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="AX3">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="AY3">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="AZ3">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="BA3">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="BB3">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="BC3">
+        <v>0.25</v>
+      </c>
+      <c r="BD3">
+        <v>0.247</v>
+      </c>
+      <c r="BE3">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="BF3">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="BG3">
+        <v>0.23</v>
+      </c>
+      <c r="BH3">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="BI3">
+        <v>0.221</v>
+      </c>
+      <c r="BJ3">
+        <v>0.216</v>
+      </c>
+      <c r="BK3">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="BL3">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="BM3">
+        <v>0.2</v>
+      </c>
+      <c r="BN3">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="BO3">
+        <v>0.191</v>
+      </c>
+      <c r="BP3">
+        <v>0.189</v>
+      </c>
+      <c r="BQ3">
+        <v>0.185</v>
+      </c>
+      <c r="BR3">
+        <v>0.18</v>
+      </c>
+      <c r="BS3">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="BT3">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="BU3">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="BV3">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="BW3">
+        <v>0.157</v>
+      </c>
+      <c r="BX3">
+        <v>0.156</v>
+      </c>
+      <c r="BY3">
+        <v>0.151</v>
+      </c>
+      <c r="BZ3">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="CA3">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="CB3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="CC3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="CD3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="CE3">
+        <v>0.13</v>
+      </c>
+      <c r="CF3">
+        <v>0.127</v>
+      </c>
+      <c r="CG3">
+        <v>0.123</v>
+      </c>
+      <c r="CH3">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="CI3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="CJ3">
+        <v>0.112</v>
+      </c>
+      <c r="CK3">
+        <v>0.11</v>
+      </c>
+      <c r="CL3">
+        <v>0.105</v>
+      </c>
+      <c r="CM3">
+        <v>0.104</v>
+      </c>
+      <c r="CN3">
+        <v>0.1</v>
+      </c>
+      <c r="CO3">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="CP3">
+        <v>9.4E-2</v>
+      </c>
+      <c r="CQ3">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="CR3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="CS3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="CT3">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="CU3">
+        <v>0.08</v>
+      </c>
+      <c r="CV3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="CW3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="CX3">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="CY3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="CZ3">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="DA3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="DB3">
+        <v>6.3E-2</v>
+      </c>
+      <c r="DC3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="DD3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="DE3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="DF3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="DG3">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="DH3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="DI3">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="DJ3">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="DK3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="DL3">
+        <v>0.04</v>
+      </c>
+      <c r="DM3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="DN3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="DO3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="DP3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="DQ3">
+        <v>3.1E-2</v>
+      </c>
+      <c r="DR3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="DS3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="DT3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="DU3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="DV3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="DW3">
+        <v>2.3E-2</v>
+      </c>
+      <c r="DX3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="DY3">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs(page_doc): finish page replacement doc
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljt12138\Desktop\oslab\sim_ran\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FB6414-EF4D-43E9-90B9-76E31856C651}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C675E8F-2524-4DDB-874E-79CE45DC1575}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="3" xr2:uid="{5F17E777-6804-43E9-9C86-08DF6650385B}"/>
   </bookViews>
@@ -11035,190 +11035,190 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>4552137</c:v>
+                  <c:v>3939190</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2365168</c:v>
+                  <c:v>2464409</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1580545</c:v>
+                  <c:v>1801156</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1176374</c:v>
+                  <c:v>1256774</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>855965</c:v>
+                  <c:v>988435</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>644607</c:v>
+                  <c:v>743741</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>475481</c:v>
+                  <c:v>564787</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>336963</c:v>
+                  <c:v>417507</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>258462</c:v>
+                  <c:v>288035</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>190063</c:v>
+                  <c:v>215025</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>140995</c:v>
+                  <c:v>163189</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>124681</c:v>
+                  <c:v>132262</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105908</c:v>
+                  <c:v>111415</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96102</c:v>
+                  <c:v>100455</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>88188</c:v>
+                  <c:v>91182</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>79829</c:v>
+                  <c:v>73947</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74188</c:v>
+                  <c:v>79241</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>70123</c:v>
+                  <c:v>70481</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>65149</c:v>
+                  <c:v>64354</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>60070</c:v>
+                  <c:v>59123</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>56522</c:v>
+                  <c:v>54708</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52042</c:v>
+                  <c:v>51334</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>47566</c:v>
+                  <c:v>46816</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43757</c:v>
+                  <c:v>42322</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41956</c:v>
+                  <c:v>37589</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39010</c:v>
+                  <c:v>36458</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>34901</c:v>
+                  <c:v>36024</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>33929</c:v>
+                  <c:v>34875</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>30790</c:v>
+                  <c:v>29696</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>28399</c:v>
+                  <c:v>27858</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>27766</c:v>
+                  <c:v>26480</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25023</c:v>
+                  <c:v>21088</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>23346</c:v>
+                  <c:v>22784</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>23100</c:v>
+                  <c:v>24123</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>21403</c:v>
+                  <c:v>18009</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16470</c:v>
+                  <c:v>19382</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>15612</c:v>
+                  <c:v>18091</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>16359</c:v>
+                  <c:v>16276</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>16968</c:v>
+                  <c:v>11556</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>15741</c:v>
+                  <c:v>14097</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13437</c:v>
+                  <c:v>13199</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>13658</c:v>
+                  <c:v>13834</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9761</c:v>
+                  <c:v>10326</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9031</c:v>
+                  <c:v>7431</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7204</c:v>
+                  <c:v>9023</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6924</c:v>
+                  <c:v>9341</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6027</c:v>
+                  <c:v>5938</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6957</c:v>
+                  <c:v>5182</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5129</c:v>
+                  <c:v>6283</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4226</c:v>
+                  <c:v>5167</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4330</c:v>
+                  <c:v>5876</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3042</c:v>
+                  <c:v>2901</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3930</c:v>
+                  <c:v>3186</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3573</c:v>
+                  <c:v>3503</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3160</c:v>
+                  <c:v>4004</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1851</c:v>
+                  <c:v>2672</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1854</c:v>
+                  <c:v>2405</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2086</c:v>
+                  <c:v>2455</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2104</c:v>
+                  <c:v>1169</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1612</c:v>
+                  <c:v>1178</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1039</c:v>
+                  <c:v>1574</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1204</c:v>
+                  <c:v>1167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12103,199 +12103,198 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet4!$R$2:$R$63</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>Sheet4!$R$1:$R$62</c:f>
+              <c:strCache>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
+                  <c:v>memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -19688,16 +19687,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>509015</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>148940</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209181</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>59315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>540304</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>86100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>184354</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>174003</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19724,16 +19723,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>415087</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>31456</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>353436</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>62281</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>348868</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>106675</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>305713</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>137500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25395,8 +25394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB417EB6-DEDC-453C-AF1F-A7ED4C772206}">
   <dimension ref="A1:AX63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN10" zoomScale="166" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2:AX63"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="V63" sqref="V63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -25409,7 +25408,7 @@
     <col min="15" max="16" width="9.4140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.75" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.4140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.4140625" customWidth="1"/>
     <col min="22" max="22" width="9.4140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.4140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.4140625" bestFit="1" customWidth="1"/>
@@ -25548,10 +25547,7 @@
         <v>2</v>
       </c>
       <c r="S2">
-        <v>4552137</v>
-      </c>
-      <c r="T2">
-        <v>5643523</v>
+        <v>3939190</v>
       </c>
       <c r="V2">
         <v>4679521</v>
@@ -25654,10 +25650,7 @@
         <v>3</v>
       </c>
       <c r="S3">
-        <v>2365168</v>
-      </c>
-      <c r="T3">
-        <v>7829738</v>
+        <v>2464409</v>
       </c>
       <c r="V3">
         <v>2510116</v>
@@ -25760,10 +25753,7 @@
         <v>4</v>
       </c>
       <c r="S4">
-        <v>1580545</v>
-      </c>
-      <c r="T4">
-        <v>8615413</v>
+        <v>1801156</v>
       </c>
       <c r="V4">
         <v>1572935</v>
@@ -25866,10 +25856,7 @@
         <v>5</v>
       </c>
       <c r="S5">
-        <v>1176374</v>
-      </c>
-      <c r="T5">
-        <v>9018064</v>
+        <v>1256774</v>
       </c>
       <c r="V5">
         <v>1026107</v>
@@ -25972,10 +25959,7 @@
         <v>6</v>
       </c>
       <c r="S6">
-        <v>855965</v>
-      </c>
-      <c r="T6">
-        <v>9338803</v>
+        <v>988435</v>
       </c>
       <c r="V6">
         <v>759442</v>
@@ -26078,10 +26062,7 @@
         <v>7</v>
       </c>
       <c r="S7">
-        <v>644607</v>
-      </c>
-      <c r="T7">
-        <v>9550333</v>
+        <v>743741</v>
       </c>
       <c r="V7">
         <v>563918</v>
@@ -26184,10 +26165,7 @@
         <v>8</v>
       </c>
       <c r="S8">
-        <v>475481</v>
-      </c>
-      <c r="T8">
-        <v>9718671</v>
+        <v>564787</v>
       </c>
       <c r="V8">
         <v>384085</v>
@@ -26290,10 +26268,7 @@
         <v>9</v>
       </c>
       <c r="S9">
-        <v>336963</v>
-      </c>
-      <c r="T9">
-        <v>9857625</v>
+        <v>417507</v>
       </c>
       <c r="V9">
         <v>274794</v>
@@ -26396,10 +26371,7 @@
         <v>10</v>
       </c>
       <c r="S10">
-        <v>258462</v>
-      </c>
-      <c r="T10">
-        <v>9936828</v>
+        <v>288035</v>
       </c>
       <c r="V10">
         <v>210487</v>
@@ -26502,10 +26474,7 @@
         <v>11</v>
       </c>
       <c r="S11">
-        <v>190063</v>
-      </c>
-      <c r="T11">
-        <v>10005101</v>
+        <v>215025</v>
       </c>
       <c r="V11">
         <v>149511</v>
@@ -26608,10 +26577,7 @@
         <v>12</v>
       </c>
       <c r="S12">
-        <v>140995</v>
-      </c>
-      <c r="T12">
-        <v>10053805</v>
+        <v>163189</v>
       </c>
       <c r="V12">
         <v>115097</v>
@@ -26714,10 +26680,7 @@
         <v>13</v>
       </c>
       <c r="S13">
-        <v>124681</v>
-      </c>
-      <c r="T13">
-        <v>10070561</v>
+        <v>132262</v>
       </c>
       <c r="V13">
         <v>105248</v>
@@ -26820,10 +26783,7 @@
         <v>14</v>
       </c>
       <c r="S14">
-        <v>105908</v>
-      </c>
-      <c r="T14">
-        <v>10088976</v>
+        <v>111415</v>
       </c>
       <c r="V14">
         <v>89064</v>
@@ -26926,10 +26886,7 @@
         <v>15</v>
       </c>
       <c r="S15">
-        <v>96102</v>
-      </c>
-      <c r="T15">
-        <v>10098366</v>
+        <v>100455</v>
       </c>
       <c r="V15">
         <v>80794</v>
@@ -27032,10 +26989,7 @@
         <v>16</v>
       </c>
       <c r="S16">
-        <v>88188</v>
-      </c>
-      <c r="T16">
-        <v>10106478</v>
+        <v>91182</v>
       </c>
       <c r="V16">
         <v>78874</v>
@@ -27138,10 +27092,7 @@
         <v>17</v>
       </c>
       <c r="S17">
-        <v>79829</v>
-      </c>
-      <c r="T17">
-        <v>10114943</v>
+        <v>73947</v>
       </c>
       <c r="V17">
         <v>65541</v>
@@ -27244,10 +27195,7 @@
         <v>18</v>
       </c>
       <c r="S18">
-        <v>74188</v>
-      </c>
-      <c r="T18">
-        <v>10120690</v>
+        <v>79241</v>
       </c>
       <c r="V18">
         <v>66507</v>
@@ -27350,10 +27298,7 @@
         <v>19</v>
       </c>
       <c r="S19">
-        <v>70123</v>
-      </c>
-      <c r="T19">
-        <v>10124687</v>
+        <v>70481</v>
       </c>
       <c r="V19">
         <v>63354</v>
@@ -27456,10 +27401,7 @@
         <v>20</v>
       </c>
       <c r="S20">
-        <v>65149</v>
-      </c>
-      <c r="T20">
-        <v>10129761</v>
+        <v>64354</v>
       </c>
       <c r="V20">
         <v>51097</v>
@@ -27562,10 +27504,7 @@
         <v>21</v>
       </c>
       <c r="S21">
-        <v>60070</v>
-      </c>
-      <c r="T21">
-        <v>10135320</v>
+        <v>59123</v>
       </c>
       <c r="V21">
         <v>56164</v>
@@ -27668,10 +27607,7 @@
         <v>22</v>
       </c>
       <c r="S22">
-        <v>56522</v>
-      </c>
-      <c r="T22">
-        <v>10137266</v>
+        <v>54708</v>
       </c>
       <c r="V22">
         <v>50517</v>
@@ -27774,10 +27710,7 @@
         <v>23</v>
       </c>
       <c r="S23">
-        <v>52042</v>
-      </c>
-      <c r="T23">
-        <v>10143098</v>
+        <v>51334</v>
       </c>
       <c r="V23">
         <v>43991</v>
@@ -27880,10 +27813,7 @@
         <v>24</v>
       </c>
       <c r="S24">
-        <v>47566</v>
-      </c>
-      <c r="T24">
-        <v>10147238</v>
+        <v>46816</v>
       </c>
       <c r="V24">
         <v>42918</v>
@@ -27986,10 +27916,7 @@
         <v>25</v>
       </c>
       <c r="S25">
-        <v>43757</v>
-      </c>
-      <c r="T25">
-        <v>10150821</v>
+        <v>42322</v>
       </c>
       <c r="V25">
         <v>40706</v>
@@ -28092,10 +28019,7 @@
         <v>26</v>
       </c>
       <c r="S26">
-        <v>41956</v>
-      </c>
-      <c r="T26">
-        <v>10152406</v>
+        <v>37589</v>
       </c>
       <c r="V26">
         <v>30998</v>
@@ -28198,10 +28122,7 @@
         <v>27</v>
       </c>
       <c r="S27">
-        <v>39010</v>
-      </c>
-      <c r="T27">
-        <v>10155894</v>
+        <v>36458</v>
       </c>
       <c r="V27">
         <v>34698</v>
@@ -28304,10 +28225,7 @@
         <v>28</v>
       </c>
       <c r="S28">
-        <v>34901</v>
-      </c>
-      <c r="T28">
-        <v>10160477</v>
+        <v>36024</v>
       </c>
       <c r="V28">
         <v>31038</v>
@@ -28410,10 +28328,7 @@
         <v>29</v>
       </c>
       <c r="S29">
-        <v>33929</v>
-      </c>
-      <c r="T29">
-        <v>10161549</v>
+        <v>34875</v>
       </c>
       <c r="V29">
         <v>31913</v>
@@ -28516,10 +28431,7 @@
         <v>30</v>
       </c>
       <c r="S30">
-        <v>30790</v>
-      </c>
-      <c r="T30">
-        <v>10163722</v>
+        <v>29696</v>
       </c>
       <c r="V30">
         <v>29560</v>
@@ -28622,10 +28534,7 @@
         <v>31</v>
       </c>
       <c r="S31">
-        <v>28399</v>
-      </c>
-      <c r="T31">
-        <v>10166223</v>
+        <v>27858</v>
       </c>
       <c r="V31">
         <v>27302</v>
@@ -28728,10 +28637,7 @@
         <v>32</v>
       </c>
       <c r="S32">
-        <v>27766</v>
-      </c>
-      <c r="T32">
-        <v>10166826</v>
+        <v>26480</v>
       </c>
       <c r="V32">
         <v>25020</v>
@@ -28834,10 +28740,7 @@
         <v>33</v>
       </c>
       <c r="S33">
-        <v>25023</v>
-      </c>
-      <c r="T33">
-        <v>10170189</v>
+        <v>21088</v>
       </c>
       <c r="V33">
         <v>23169</v>
@@ -28940,10 +28843,7 @@
         <v>34</v>
       </c>
       <c r="S34">
-        <v>23346</v>
-      </c>
-      <c r="T34">
-        <v>10171124</v>
+        <v>22784</v>
       </c>
       <c r="V34">
         <v>21629</v>
@@ -29046,10 +28946,7 @@
         <v>35</v>
       </c>
       <c r="S35">
-        <v>23100</v>
-      </c>
-      <c r="T35">
-        <v>10172762</v>
+        <v>24123</v>
       </c>
       <c r="V35">
         <v>20763</v>
@@ -29152,10 +29049,7 @@
         <v>36</v>
       </c>
       <c r="S36">
-        <v>21403</v>
-      </c>
-      <c r="T36">
-        <v>10173207</v>
+        <v>18009</v>
       </c>
       <c r="V36">
         <v>19989</v>
@@ -29258,10 +29152,7 @@
         <v>37</v>
       </c>
       <c r="S37">
-        <v>16470</v>
-      </c>
-      <c r="T37">
-        <v>10178066</v>
+        <v>19382</v>
       </c>
       <c r="V37">
         <v>15883</v>
@@ -29364,10 +29255,7 @@
         <v>38</v>
       </c>
       <c r="S38">
-        <v>15612</v>
-      </c>
-      <c r="T38">
-        <v>10178746</v>
+        <v>18091</v>
       </c>
       <c r="V38">
         <v>14730</v>
@@ -29470,10 +29358,7 @@
         <v>39</v>
       </c>
       <c r="S39">
-        <v>16359</v>
-      </c>
-      <c r="T39">
-        <v>10178607</v>
+        <v>16276</v>
       </c>
       <c r="V39">
         <v>14824</v>
@@ -29576,10 +29461,7 @@
         <v>40</v>
       </c>
       <c r="S40">
-        <v>16968</v>
-      </c>
-      <c r="T40">
-        <v>10177588</v>
+        <v>11556</v>
       </c>
       <c r="V40">
         <v>12650</v>
@@ -29682,10 +29564,7 @@
         <v>41</v>
       </c>
       <c r="S41">
-        <v>15741</v>
-      </c>
-      <c r="T41">
-        <v>10178457</v>
+        <v>14097</v>
       </c>
       <c r="V41">
         <v>12733</v>
@@ -29788,10 +29667,7 @@
         <v>42</v>
       </c>
       <c r="S42">
-        <v>13437</v>
-      </c>
-      <c r="T42">
-        <v>10181441</v>
+        <v>13199</v>
       </c>
       <c r="V42">
         <v>12090</v>
@@ -29894,10 +29770,7 @@
         <v>43</v>
       </c>
       <c r="S43">
-        <v>13658</v>
-      </c>
-      <c r="T43">
-        <v>10181662</v>
+        <v>13834</v>
       </c>
       <c r="V43">
         <v>11103</v>
@@ -30000,10 +29873,7 @@
         <v>44</v>
       </c>
       <c r="S44">
-        <v>9761</v>
-      </c>
-      <c r="T44">
-        <v>10185145</v>
+        <v>10326</v>
       </c>
       <c r="V44">
         <v>11072</v>
@@ -30106,10 +29976,7 @@
         <v>45</v>
       </c>
       <c r="S45">
-        <v>9031</v>
-      </c>
-      <c r="T45">
-        <v>10185953</v>
+        <v>7431</v>
       </c>
       <c r="V45">
         <v>8953</v>
@@ -30212,10 +30079,7 @@
         <v>46</v>
       </c>
       <c r="S46">
-        <v>7204</v>
-      </c>
-      <c r="T46">
-        <v>10186874</v>
+        <v>9023</v>
       </c>
       <c r="V46">
         <v>11024</v>
@@ -30318,10 +30182,7 @@
         <v>47</v>
       </c>
       <c r="S47">
-        <v>6924</v>
-      </c>
-      <c r="T47">
-        <v>10187952</v>
+        <v>9341</v>
       </c>
       <c r="V47">
         <v>8301</v>
@@ -30424,10 +30285,7 @@
         <v>48</v>
       </c>
       <c r="S48">
-        <v>6027</v>
-      </c>
-      <c r="T48">
-        <v>10188527</v>
+        <v>5938</v>
       </c>
       <c r="V48">
         <v>5845</v>
@@ -30530,10 +30388,7 @@
         <v>49</v>
       </c>
       <c r="S49">
-        <v>6957</v>
-      </c>
-      <c r="T49">
-        <v>10187721</v>
+        <v>5182</v>
       </c>
       <c r="V49">
         <v>6004</v>
@@ -30636,10 +30491,7 @@
         <v>50</v>
       </c>
       <c r="S50">
-        <v>5129</v>
-      </c>
-      <c r="T50">
-        <v>10188809</v>
+        <v>6283</v>
       </c>
       <c r="V50">
         <v>6406</v>
@@ -30742,10 +30594,7 @@
         <v>51</v>
       </c>
       <c r="S51">
-        <v>4226</v>
-      </c>
-      <c r="T51">
-        <v>10190636</v>
+        <v>5167</v>
       </c>
       <c r="V51">
         <v>3640</v>
@@ -30848,10 +30697,7 @@
         <v>52</v>
       </c>
       <c r="S52">
-        <v>4330</v>
-      </c>
-      <c r="T52">
-        <v>10190978</v>
+        <v>5876</v>
       </c>
       <c r="V52">
         <v>4053</v>
@@ -30954,10 +30800,7 @@
         <v>53</v>
       </c>
       <c r="S53">
-        <v>3042</v>
-      </c>
-      <c r="T53">
-        <v>10191382</v>
+        <v>2901</v>
       </c>
       <c r="V53">
         <v>3922</v>
@@ -31060,10 +30903,7 @@
         <v>54</v>
       </c>
       <c r="S54">
-        <v>3930</v>
-      </c>
-      <c r="T54">
-        <v>10190570</v>
+        <v>3186</v>
       </c>
       <c r="V54">
         <v>3964</v>
@@ -31166,10 +31006,7 @@
         <v>55</v>
       </c>
       <c r="S55">
-        <v>3573</v>
-      </c>
-      <c r="T55">
-        <v>10192015</v>
+        <v>3503</v>
       </c>
       <c r="V55">
         <v>3277</v>
@@ -31272,10 +31109,7 @@
         <v>56</v>
       </c>
       <c r="S56">
-        <v>3160</v>
-      </c>
-      <c r="T56">
-        <v>10192206</v>
+        <v>4004</v>
       </c>
       <c r="V56">
         <v>4415</v>
@@ -31378,10 +31212,7 @@
         <v>57</v>
       </c>
       <c r="S57">
-        <v>1851</v>
-      </c>
-      <c r="T57">
-        <v>10193307</v>
+        <v>2672</v>
       </c>
       <c r="V57">
         <v>1838</v>
@@ -31484,10 +31315,7 @@
         <v>58</v>
       </c>
       <c r="S58">
-        <v>1854</v>
-      </c>
-      <c r="T58">
-        <v>10193008</v>
+        <v>2405</v>
       </c>
       <c r="V58">
         <v>2143</v>
@@ -31590,10 +31418,7 @@
         <v>59</v>
       </c>
       <c r="S59">
-        <v>2086</v>
-      </c>
-      <c r="T59">
-        <v>10192222</v>
+        <v>2455</v>
       </c>
       <c r="V59">
         <v>2541</v>
@@ -31696,10 +31521,7 @@
         <v>60</v>
       </c>
       <c r="S60">
-        <v>2104</v>
-      </c>
-      <c r="T60">
-        <v>10192368</v>
+        <v>1169</v>
       </c>
       <c r="V60">
         <v>2018</v>
@@ -31802,10 +31624,7 @@
         <v>61</v>
       </c>
       <c r="S61">
-        <v>1612</v>
-      </c>
-      <c r="T61">
-        <v>10193238</v>
+        <v>1178</v>
       </c>
       <c r="V61">
         <v>1355</v>
@@ -31908,10 +31727,7 @@
         <v>62</v>
       </c>
       <c r="S62">
-        <v>1039</v>
-      </c>
-      <c r="T62">
-        <v>10193763</v>
+        <v>1574</v>
       </c>
       <c r="V62">
         <v>1247</v>
@@ -32014,10 +31830,7 @@
         <v>63</v>
       </c>
       <c r="S63">
-        <v>1204</v>
-      </c>
-      <c r="T63">
-        <v>10194074</v>
+        <v>1167</v>
       </c>
       <c r="V63">
         <v>1054</v>

</xml_diff>